<commit_message>
append messing files and adding Odds Ratio
</commit_message>
<xml_diff>
--- a/Summarise models.xlsx
+++ b/Summarise models.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://playtika-my.sharepoint.com/personal/shahars_playtika_com/Documents/Documents/GitHub/Statistics-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="450" documentId="11_F25DC773A252ABDACC104853E1DC471A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99780040-1DE5-4772-9BDF-AF27649BDE7A}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="11_F25DC773A252ABDACC104853E1DC471A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43D0BFEC-4DD0-4B29-B195-67B5CF0AC583}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1Y" sheetId="2" r:id="rId1"/>
     <sheet name="2Y" sheetId="1" r:id="rId2"/>
+    <sheet name="Risk" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
   <si>
     <t>Estimate</t>
   </si>
@@ -259,12 +260,39 @@
       <t>Female</t>
     </r>
   </si>
+  <si>
+    <t>1Y</t>
+  </si>
+  <si>
+    <t>2y</t>
+  </si>
+  <si>
+    <t>Up to March19</t>
+  </si>
+  <si>
+    <t>March19 to March 20</t>
+  </si>
+  <si>
+    <t>March20 to Feb21</t>
+  </si>
+  <si>
+    <t>From Feb21</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Odds Ratio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +313,13 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -445,10 +480,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -474,9 +511,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -496,9 +530,68 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,77 +599,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -587,11 +619,104 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -907,453 +1032,482 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D56BC0C-6107-419F-B05A-9A618735733E}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9" customWidth="1"/>
+    <col min="2" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="38"/>
-      <c r="B2" s="35" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="39"/>
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="E2" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="27">
         <v>-0.93</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="55">
         <v>0.45</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="55">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="E3" s="56"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="27">
         <v>0.49</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="55">
         <v>0.15</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="E4" s="56"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="27">
         <v>0.39</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="55">
         <v>0.18</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="55">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="E5" s="56"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="27">
         <v>-0.39</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="55">
         <v>0.1</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="55">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="E6" s="56"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="27">
         <v>-0.39</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="55">
         <v>0.19</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="55">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="E7" s="56"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="23">
         <v>0</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="57">
         <v>0.13</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="57">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="E8" s="58"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="23">
         <v>0.22</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="57">
         <v>0.15</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="57">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="E9" s="58"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="27">
         <v>0.04</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="55">
         <v>0.01</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="55">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="E10" s="56"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="27">
         <v>0.45</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="55">
         <v>0.22</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="55">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="E11" s="56"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="23">
         <v>0.2</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="57">
         <v>0.16</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="57">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="E12" s="58"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="23">
         <v>0.08</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="57">
         <v>0.05</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="57">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="E13" s="58"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="23">
         <v>-0.15</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="57">
         <v>0.18</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="57">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="E14" s="59">
+        <f>EXP(B14)</f>
+        <v>0.86070797642505781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="23">
         <v>0.05</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="57">
         <v>0.18</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="57">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="E15" s="59">
+        <f t="shared" ref="E15:E16" si="0">EXP(B15)</f>
+        <v>1.0512710963760241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16" s="30">
         <v>0.73</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>0.23</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="14">
         <v>0</v>
       </c>
+      <c r="E16" s="60">
+        <f t="shared" si="0"/>
+        <v>2.0750806076741224</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="38"/>
-      <c r="B20" s="36" t="s">
+      <c r="A20" s="39"/>
+      <c r="B20" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="28">
         <v>-0.94527000000000005</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="28">
         <v>0.44740000000000002</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="29">
         <v>3.4619999999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="41">
+      <c r="B22" s="28">
         <v>0.48551</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="28">
         <v>0.15411</v>
       </c>
-      <c r="D22" s="42">
+      <c r="D22" s="29">
         <v>1.6299999999999999E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="41">
+      <c r="B23" s="28">
         <v>0.3755</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="28">
         <v>0.18232000000000001</v>
       </c>
-      <c r="D23" s="42">
+      <c r="D23" s="29">
         <v>3.943E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="41">
+      <c r="B24" s="28">
         <v>-0.37953999999999999</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="28">
         <v>0.10172</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="29">
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="41">
+      <c r="B25" s="28">
         <v>-0.4254</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="28">
         <v>0.191</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D25" s="29">
         <v>2.5930000000000002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="22">
         <v>6.3699999999999998E-3</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="22">
         <v>0.13231999999999999</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="19">
         <v>0.96162000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="22">
         <v>0.23727999999999999</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="22">
         <v>0.15168999999999999</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="19">
         <v>0.11774999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="41">
+      <c r="B28" s="28">
         <v>3.8730000000000001E-2</v>
       </c>
-      <c r="C28" s="41">
+      <c r="C28" s="28">
         <v>1.316E-2</v>
       </c>
-      <c r="D28" s="42">
+      <c r="D28" s="29">
         <v>3.2499999999999999E-3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="41">
+      <c r="B29" s="28">
         <v>0.44175999999999999</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="28">
         <v>0.22267000000000001</v>
       </c>
-      <c r="D29" s="42">
+      <c r="D29" s="29">
         <v>4.727E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="22">
         <v>0.20347999999999999</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="22">
         <v>0.15995000000000001</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="19">
         <v>0.20330000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="30">
+      <c r="B31" s="22">
         <v>8.3909999999999998E-2</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="22">
         <v>5.1339999999999997E-2</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="19">
         <v>0.10217</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="31">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="36">
         <v>1.7E-5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="31"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="36"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="32"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D32:D34"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D16">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D32">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1366,308 +1520,337 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.54296875" style="2" customWidth="1"/>
+    <col min="2" max="4" width="9.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="9.54296875" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="44"/>
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>-0.83</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="17">
         <v>0.52</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="17">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>0.37</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="31">
         <v>0.16</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="31">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="17">
         <v>0.19</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="17">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="31">
         <v>0.1</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="31">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>0.1</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="17">
         <v>0.13</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="17">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>0.19</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="17">
         <v>0.15</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="17">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>-0.02</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="17">
         <v>0.01</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="17">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>0.08</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="17">
         <v>0.22</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="17">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>0.08</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="17">
         <v>0.16</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="17">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>-0.09</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="31">
         <v>0.05</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="31">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>0.04</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="17">
         <v>0.19</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="17">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <v>0.43</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="17">
         <v>0.27</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="17">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>-0.32</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="17">
         <v>0.22</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="17">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <v>0.17</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="17">
         <v>0.12</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="17">
         <v>0.14000000000000001</v>
       </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <v>0.38</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="31">
         <v>0.18</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="31">
         <v>0.04</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="E17" s="29">
+        <f>EXP(B17)</f>
+        <v>1.4622845894342245</v>
+      </c>
+      <c r="F17" s="49"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>0.64</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="31">
         <v>0.19</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="31">
         <v>0</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="E18" s="29">
+        <f>EXP(B18)</f>
+        <v>1.8964808793049515</v>
+      </c>
+      <c r="F18" s="49"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="33">
         <v>0.67</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="34">
         <v>0.22</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="34">
         <v>0</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="E19" s="35">
+        <f>EXP(B19)</f>
+        <v>1.9542373206359396</v>
+      </c>
+      <c r="F19" s="49"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
+      <c r="A21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="34"/>
-      <c r="B24" s="36" t="s">
+      <c r="A24" s="44"/>
+      <c r="B24" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="26" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1675,27 +1858,27 @@
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="18">
         <v>-0.32819999999999999</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="18">
         <v>0.51949999999999996</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="19">
         <v>0.52759999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B26" s="32">
         <v>0.37030000000000002</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="32">
         <v>0.1578</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="29">
         <v>1.89E-2</v>
       </c>
     </row>
@@ -1703,13 +1886,13 @@
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="18">
         <v>0.1401</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="18">
         <v>0.18629999999999999</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="19">
         <v>0.45200000000000001</v>
       </c>
     </row>
@@ -1717,13 +1900,13 @@
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B28" s="32">
         <v>-0.28299999999999997</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="32">
         <v>0.1014</v>
       </c>
-      <c r="D28" s="42">
+      <c r="D28" s="29">
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
@@ -1731,13 +1914,13 @@
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="18">
         <v>9.7299999999999998E-2</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="18">
         <v>0.1303</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="19">
         <v>0.45529999999999998</v>
       </c>
     </row>
@@ -1745,13 +1928,13 @@
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="18">
         <v>0.19789999999999999</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="18">
         <v>0.14860000000000001</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="19">
         <v>0.18310000000000001</v>
       </c>
     </row>
@@ -1759,13 +1942,13 @@
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="18">
         <v>-1.9800000000000002E-2</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="18">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="19">
         <v>0.12770000000000001</v>
       </c>
     </row>
@@ -1773,13 +1956,13 @@
       <c r="A32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="18">
         <v>7.7499999999999999E-2</v>
       </c>
-      <c r="C32" s="25">
+      <c r="C32" s="18">
         <v>0.221</v>
       </c>
-      <c r="D32" s="26">
+      <c r="D32" s="19">
         <v>0.72570000000000001</v>
       </c>
     </row>
@@ -1787,13 +1970,13 @@
       <c r="A33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="18">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="18">
         <v>0.16189999999999999</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="19">
         <v>0.60680000000000001</v>
       </c>
     </row>
@@ -1801,13 +1984,13 @@
       <c r="A34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="45">
+      <c r="B34" s="32">
         <v>-9.5399999999999999E-2</v>
       </c>
-      <c r="C34" s="45">
+      <c r="C34" s="32">
         <v>5.16E-2</v>
       </c>
-      <c r="D34" s="42">
+      <c r="D34" s="29">
         <v>6.4699999999999994E-2</v>
       </c>
     </row>
@@ -1815,13 +1998,13 @@
       <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="18">
         <v>5.5800000000000002E-2</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="18">
         <v>0.18779999999999999</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="19">
         <v>0.76659999999999995</v>
       </c>
     </row>
@@ -1829,13 +2012,13 @@
       <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="18">
         <v>0.42080000000000001</v>
       </c>
-      <c r="C36" s="25">
+      <c r="C36" s="18">
         <v>0.2671</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="19">
         <v>0.11509999999999999</v>
       </c>
     </row>
@@ -1843,13 +2026,13 @@
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B37" s="18">
         <v>-0.32029999999999997</v>
       </c>
-      <c r="C37" s="25">
+      <c r="C37" s="18">
         <v>0.218</v>
       </c>
-      <c r="D37" s="26">
+      <c r="D37" s="19">
         <v>0.14180000000000001</v>
       </c>
     </row>
@@ -1857,13 +2040,13 @@
       <c r="A38" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B38" s="18">
         <v>0.14580000000000001</v>
       </c>
-      <c r="C38" s="25">
+      <c r="C38" s="18">
         <v>0.1158</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="19">
         <v>0.20780000000000001</v>
       </c>
     </row>
@@ -1871,9 +2054,9 @@
       <c r="A39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="50">
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="47">
         <v>3.3000000000000003E-5</v>
       </c>
     </row>
@@ -1881,41 +2064,129 @@
       <c r="A40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="50"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="47"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="49"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="48"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="8">
+  <mergeCells count="7">
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="B1:E1"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B39:C41"/>
     <mergeCell ref="D39:D41"/>
-    <mergeCell ref="B1:D1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D19">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:D39">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E61670A-EC09-4D32-BBF9-D4AD18A0D1AA}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="42"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="39"/>
+      <c r="B2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="51">
+        <v>0.58945999999999998</v>
+      </c>
+      <c r="C3" s="52">
+        <v>0.4204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="51">
+        <v>0.55259999999999998</v>
+      </c>
+      <c r="C4" s="52">
+        <v>0.51346999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="51">
+        <v>0.60158</v>
+      </c>
+      <c r="C5" s="52">
+        <v>0.57918000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="53">
+        <v>0.74939999999999996</v>
+      </c>
+      <c r="C6" s="54">
+        <v>0.58667999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add presentation for Idit
</commit_message>
<xml_diff>
--- a/Summarise models.xlsx
+++ b/Summarise models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edena\Documents\GitHub\Statistics-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F6FE08-CFBC-456D-8B28-3D9627A93529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E79FF7-2B68-4E11-9B04-C1F52C18BDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="2" r:id="rId1"/>
@@ -437,6 +437,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,18 +477,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D56BC0C-6107-419F-B05A-9A618735733E}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33:K57"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -778,63 +778,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="28"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="28"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
-      <c r="H5" s="34" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="H5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="33"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="37"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -847,7 +847,7 @@
       <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="35"/>
+      <c r="H6" s="39"/>
       <c r="I6" s="9" t="s">
         <v>0</v>
       </c>
@@ -1465,14 +1465,14 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
       <c r="H27" s="16" t="s">
         <v>32</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="9" t="s">
         <v>0</v>
       </c>
@@ -1630,14 +1630,14 @@
       <c r="D33" s="12">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="H33" s="34" t="s">
+      <c r="H33" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I33" s="32" t="s">
+      <c r="I33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="J33" s="32"/>
-      <c r="K33" s="33"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="37"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -1655,7 +1655,7 @@
       <c r="D34" s="12">
         <v>3.6479999999999999E-2</v>
       </c>
-      <c r="H34" s="35"/>
+      <c r="H34" s="39"/>
       <c r="I34" s="9" t="s">
         <v>0</v>
       </c>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
-      <c r="D44" s="29">
+      <c r="D44" s="33">
         <v>0</v>
       </c>
       <c r="H44" s="17" t="s">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
-      <c r="D45" s="29"/>
+      <c r="D45" s="33"/>
       <c r="H45" s="17" t="s">
         <v>29</v>
       </c>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
-      <c r="D46" s="30"/>
+      <c r="D46" s="34"/>
       <c r="H46" s="17" t="s">
         <v>30</v>
       </c>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="I55" s="19"/>
       <c r="J55" s="19"/>
-      <c r="K55" s="29">
+      <c r="K55" s="33">
         <v>3.2000000000000002E-3</v>
       </c>
       <c r="M55" s="1"/>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="I56" s="19"/>
       <c r="J56" s="19"/>
-      <c r="K56" s="29"/>
+      <c r="K56" s="33"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
     </row>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="I57" s="21"/>
       <c r="J57" s="21"/>
-      <c r="K57" s="30"/>
+      <c r="K57" s="34"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
     </row>
@@ -2193,7 +2193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB9A3F7-BE72-43C3-BC6B-D24E893A6BDB}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2210,23 +2210,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="32" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
-      <c r="H23" s="29">
+      <c r="H23" s="33">
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
@@ -2771,7 +2771,7 @@
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="29"/>
+      <c r="H24" s="33"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="30"/>
+      <c r="H25" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2820,16 +2820,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="33"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
@@ -2841,10 +2841,10 @@
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="29">
         <v>0.59314</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="30">
         <v>0.378</v>
       </c>
     </row>
@@ -2852,10 +2852,10 @@
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="29">
         <v>0.55674999999999997</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="30">
         <v>0.54862999999999995</v>
       </c>
     </row>
@@ -2863,10 +2863,10 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="29">
         <v>0.60360000000000003</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="30">
         <v>0.55262</v>
       </c>
     </row>
@@ -2874,10 +2874,10 @@
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="31">
         <v>0.74299999999999999</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="32">
         <v>0.53993000000000002</v>
       </c>
     </row>

</xml_diff>